<commit_message>
Agregado sistema de puntajes
</commit_message>
<xml_diff>
--- a/comparacion.xlsx
+++ b/comparacion.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:C11"/>
+  <dimension ref="A1:F11"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -449,6 +449,17 @@
           <t>REDMONK</t>
         </is>
       </c>
+      <c r="D1" s="1" t="inlineStr"/>
+      <c r="E1" s="1" t="inlineStr">
+        <is>
+          <t>Puntaje</t>
+        </is>
+      </c>
+      <c r="F1" s="1" t="inlineStr">
+        <is>
+          <t>Lenguaje</t>
+        </is>
+      </c>
     </row>
     <row r="2">
       <c r="A2" t="inlineStr">
@@ -466,6 +477,15 @@
           <t>JavaScript</t>
         </is>
       </c>
+      <c r="D2" t="inlineStr"/>
+      <c r="E2" t="n">
+        <v>29</v>
+      </c>
+      <c r="F2" t="inlineStr">
+        <is>
+          <t>Python</t>
+        </is>
+      </c>
     </row>
     <row r="3">
       <c r="A3" t="inlineStr">
@@ -483,6 +503,15 @@
           <t>Python</t>
         </is>
       </c>
+      <c r="D3" t="inlineStr"/>
+      <c r="E3" t="n">
+        <v>26</v>
+      </c>
+      <c r="F3" t="inlineStr">
+        <is>
+          <t>Java</t>
+        </is>
+      </c>
     </row>
     <row r="4">
       <c r="A4" t="inlineStr">
@@ -500,6 +529,15 @@
           <t>Java</t>
         </is>
       </c>
+      <c r="D4" t="inlineStr"/>
+      <c r="E4" t="n">
+        <v>25</v>
+      </c>
+      <c r="F4" t="inlineStr">
+        <is>
+          <t>JavaScript</t>
+        </is>
+      </c>
     </row>
     <row r="5">
       <c r="A5" t="inlineStr">
@@ -517,6 +555,15 @@
           <t>PHP</t>
         </is>
       </c>
+      <c r="D5" t="inlineStr"/>
+      <c r="E5" t="n">
+        <v>21</v>
+      </c>
+      <c r="F5" t="inlineStr">
+        <is>
+          <t>C#</t>
+        </is>
+      </c>
     </row>
     <row r="6">
       <c r="A6" t="inlineStr">
@@ -534,6 +581,15 @@
           <t>C#</t>
         </is>
       </c>
+      <c r="D6" t="inlineStr"/>
+      <c r="E6" t="n">
+        <v>16</v>
+      </c>
+      <c r="F6" t="inlineStr">
+        <is>
+          <t>PHP</t>
+        </is>
+      </c>
     </row>
     <row r="7">
       <c r="A7" t="inlineStr">
@@ -551,6 +607,15 @@
           <t>TypeScript</t>
         </is>
       </c>
+      <c r="D7" t="inlineStr"/>
+      <c r="E7" t="n">
+        <v>10</v>
+      </c>
+      <c r="F7" t="inlineStr">
+        <is>
+          <t>R</t>
+        </is>
+      </c>
     </row>
     <row r="8">
       <c r="A8" t="inlineStr">
@@ -568,6 +633,15 @@
           <t>Ruby</t>
         </is>
       </c>
+      <c r="D8" t="inlineStr"/>
+      <c r="E8" t="n">
+        <v>9</v>
+      </c>
+      <c r="F8" t="inlineStr">
+        <is>
+          <t>Go</t>
+        </is>
+      </c>
     </row>
     <row r="9">
       <c r="A9" t="inlineStr">
@@ -585,6 +659,15 @@
           <t>Swift</t>
         </is>
       </c>
+      <c r="D9" t="inlineStr"/>
+      <c r="E9" t="n">
+        <v>9</v>
+      </c>
+      <c r="F9" t="inlineStr">
+        <is>
+          <t>TypeScript</t>
+        </is>
+      </c>
     </row>
     <row r="10">
       <c r="A10" t="inlineStr">
@@ -602,6 +685,15 @@
           <t>Go</t>
         </is>
       </c>
+      <c r="D10" t="inlineStr"/>
+      <c r="E10" t="n">
+        <v>7</v>
+      </c>
+      <c r="F10" t="inlineStr">
+        <is>
+          <t>Rust</t>
+        </is>
+      </c>
     </row>
     <row r="11">
       <c r="A11" t="inlineStr">
@@ -617,6 +709,15 @@
       <c r="C11" t="inlineStr">
         <is>
           <t>R</t>
+        </is>
+      </c>
+      <c r="D11" t="inlineStr"/>
+      <c r="E11" t="n">
+        <v>7</v>
+      </c>
+      <c r="F11" t="inlineStr">
+        <is>
+          <t>Swift</t>
         </is>
       </c>
     </row>

</xml_diff>